<commit_message>
add person flow and Hubei Data
</commit_message>
<xml_diff>
--- a/武汉人口外流统计.xlsx
+++ b/武汉人口外流统计.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\86150\.spyder-py3\projects\MCM-ICM2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29F0F7EA-F6E0-4DF3-8374-B689793CB646}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44D75FF-9591-4DE6-854D-722CA99FD9EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -348,7 +348,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -377,6 +377,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1233,108 +1236,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10" t="s">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10" t="s">
+      <c r="J1" s="11"/>
+      <c r="K1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10" t="s">
+      <c r="L1" s="11"/>
+      <c r="M1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10" t="s">
+      <c r="N1" s="11"/>
+      <c r="O1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10" t="s">
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10" t="s">
+      <c r="R1" s="11"/>
+      <c r="S1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10" t="s">
+      <c r="T1" s="11"/>
+      <c r="U1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10" t="s">
+      <c r="V1" s="11"/>
+      <c r="W1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10" t="s">
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10" t="s">
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10" t="s">
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10" t="s">
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10" t="s">
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10" t="s">
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10" t="s">
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AL1" s="10"/>
-      <c r="AM1" s="10" t="s">
+      <c r="AL1" s="11"/>
+      <c r="AM1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10" t="s">
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="AP1" s="10"/>
-      <c r="AQ1" s="10" t="s">
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="10" t="s">
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="AT1" s="10"/>
-      <c r="AU1" s="10" t="s">
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="AV1" s="10"/>
+      <c r="AV1" s="11"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
@@ -5462,6 +5465,21 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="AC1:AD1"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AU1:AV1"/>
@@ -5472,21 +5490,6 @@
     <mergeCell ref="AQ1:AR1"/>
     <mergeCell ref="AS1:AT1"/>
     <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AA1:AB1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5498,8 +5501,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:BL57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -5509,140 +5512,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10" t="s">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10" t="s">
+      <c r="J1" s="11"/>
+      <c r="K1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10" t="s">
+      <c r="L1" s="11"/>
+      <c r="M1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10" t="s">
+      <c r="N1" s="11"/>
+      <c r="O1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10" t="s">
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10" t="s">
+      <c r="R1" s="11"/>
+      <c r="S1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10" t="s">
+      <c r="T1" s="11"/>
+      <c r="U1" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10" t="s">
+      <c r="V1" s="11"/>
+      <c r="W1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10" t="s">
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10" t="s">
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10" t="s">
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10" t="s">
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10" t="s">
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10" t="s">
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10" t="s">
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="AL1" s="10"/>
-      <c r="AM1" s="10" t="s">
+      <c r="AL1" s="11"/>
+      <c r="AM1" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10" t="s">
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="AP1" s="10"/>
-      <c r="AQ1" s="10" t="s">
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="10" t="s">
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="AT1" s="10"/>
-      <c r="AU1" s="10" t="s">
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AV1" s="10"/>
-      <c r="AW1" s="10" t="s">
+      <c r="AV1" s="11"/>
+      <c r="AW1" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AX1" s="10"/>
-      <c r="AY1" s="10" t="s">
+      <c r="AX1" s="11"/>
+      <c r="AY1" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AZ1" s="10"/>
-      <c r="BA1" s="10" t="s">
+      <c r="AZ1" s="11"/>
+      <c r="BA1" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="BB1" s="10"/>
-      <c r="BC1" s="10" t="s">
+      <c r="BB1" s="11"/>
+      <c r="BC1" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="BD1" s="10"/>
-      <c r="BE1" s="10" t="s">
+      <c r="BD1" s="11"/>
+      <c r="BE1" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="BF1" s="10"/>
-      <c r="BG1" s="10" t="s">
+      <c r="BF1" s="11"/>
+      <c r="BG1" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="BH1" s="10"/>
-      <c r="BI1" s="10" t="s">
+      <c r="BH1" s="11"/>
+      <c r="BI1" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="BJ1" s="10"/>
-      <c r="BK1" s="10" t="s">
+      <c r="BJ1" s="11"/>
+      <c r="BK1" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="BL1" s="10"/>
+      <c r="BL1" s="11"/>
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
       <c r="C2" s="7" t="s">
         <v>32</v>
       </c>
@@ -11001,6 +11004,16 @@
       <c r="BL25" s="7">
         <f t="shared" si="30"/>
         <v>7.0270611240774619E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B26" s="10">
+        <f>AVERAGE(B3:B25)</f>
+        <v>217.39130434782612</v>
+      </c>
+      <c r="C26" s="5">
+        <f>AVERAGE(C3:C25)</f>
+        <v>0.66757826086956529</v>
       </c>
     </row>
     <row r="27" spans="1:64" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -11035,6 +11048,27 @@
     <row r="57" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="BG1:BH1"/>
+    <mergeCell ref="BI1:BJ1"/>
+    <mergeCell ref="BK1:BL1"/>
+    <mergeCell ref="AU1:AV1"/>
+    <mergeCell ref="AW1:AX1"/>
+    <mergeCell ref="AY1:AZ1"/>
+    <mergeCell ref="BA1:BB1"/>
+    <mergeCell ref="BC1:BD1"/>
+    <mergeCell ref="BE1:BF1"/>
+    <mergeCell ref="AS1:AT1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AM1:AN1"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AQ1:AR1"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -11047,29 +11081,40 @@
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="S1:T1"/>
-    <mergeCell ref="AS1:AT1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="AI1:AJ1"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AM1:AN1"/>
-    <mergeCell ref="AO1:AP1"/>
-    <mergeCell ref="AQ1:AR1"/>
-    <mergeCell ref="BG1:BH1"/>
-    <mergeCell ref="BI1:BJ1"/>
-    <mergeCell ref="BK1:BL1"/>
-    <mergeCell ref="AU1:AV1"/>
-    <mergeCell ref="AW1:AX1"/>
-    <mergeCell ref="AY1:AZ1"/>
-    <mergeCell ref="BA1:BB1"/>
-    <mergeCell ref="BC1:BD1"/>
-    <mergeCell ref="BE1:BF1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="B3:B26">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6385CE89-BCDB-4A60-ADA6-385EDC5A9F41}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6385CE89-BCDB-4A60-ADA6-385EDC5A9F41}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B3:B26</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>